<commit_message>
Added missing transportation costs
</commit_message>
<xml_diff>
--- a/input_data/deliveries.xlsx
+++ b/input_data/deliveries.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christinesorli/Chris-Tora-master/input_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristinehagen/PycharmProjects/chris/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6B4582-5832-2F41-8A89-636E709EC97C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="52540" yWindow="2240" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Delivery" sheetId="7" r:id="rId1"/>
@@ -25,15 +26,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Delivery!$A$1:$F$1</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -42,12 +40,15 @@
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1977" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1986" uniqueCount="73">
   <si>
     <t>Vendor</t>
   </si>
@@ -264,11 +265,14 @@
   <si>
     <t>2-3</t>
   </si>
+  <si>
+    <t>Ops: Kristine lagt til</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="7" formatCode="&quot;kr&quot;\ #,##0.00;\-&quot;kr&quot;\ #,##0.00"/>
   </numFmts>
@@ -357,14 +361,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F100" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F100" headerRowDxfId="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="Vendor"/>
-    <tableColumn id="7" name="Delivery ID"/>
-    <tableColumn id="2" name="Sales Quantity (Selected period)"/>
-    <tableColumn id="3" name="Product"/>
-    <tableColumn id="4" name="Purchase Price" dataDxfId="0"/>
-    <tableColumn id="5" name="Arrival Date"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Vendor"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Delivery ID"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Sales Quantity (Selected period)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Product"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Purchase Price" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Arrival Date"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -666,7 +670,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -841,8 +845,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1">
-    <sortState ref="A2:F28">
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F28">
       <sortCondition ref="A1:A28"/>
     </sortState>
   </autoFilter>
@@ -851,11 +855,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -863,9 +867,10 @@
     <col min="1" max="1" width="18.33203125" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="18"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -876,7 +881,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
@@ -887,7 +892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
@@ -898,7 +903,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>8</v>
       </c>
@@ -909,7 +914,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>8</v>
       </c>
@@ -920,7 +925,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>8</v>
       </c>
@@ -929,6 +934,48 @@
       </c>
       <c r="C6">
         <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="13">
+        <v>14</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="13">
+        <v>14</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -937,11 +984,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -967,7 +1014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2497,7 +2544,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3995,7 +4042,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5357,7 +5404,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6136,7 +6183,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D325"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8761,7 +8808,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>